<commit_message>
Agrego marco de trabajo para talleristas de la guía de subnacionales y visibilizo especificaciones en el índice.
</commit_message>
<xml_diff>
--- a/docs/datasets-especificaciones/denuncias-campos.xlsx
+++ b/docs/datasets-especificaciones/denuncias-campos.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,12 +494,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Persona</t>
+          <t>Denuncia</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>denunciante_id</t>
+          <t>denuncia_id</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -509,18 +509,17 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Identificador de la persona que denuncia.</t>
+          <t>Identificador de la denuncia realizada.</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>23668249</t>
+          <t>3384556</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>popolo:Person
- schema:Person</t>
+          <t>schema:Thing</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
@@ -533,30 +532,34 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Persona</t>
+          <t>Denuncia</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>denunciante_id_tipo</t>
+          <t>denuncia_fecha</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>alfanumerico</t>
+          <t>fecha</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Tipo de identificación de la persona que denuncia.</t>
+          <t>Fecha de la denuncia.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>DNI</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr"/>
+          <t>2019-03-12</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>schema:Thing</t>
+        </is>
+      </c>
       <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
@@ -567,33 +570,32 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Persona</t>
+          <t>Denuncia</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>denunciante_nombre</t>
+          <t>denuncia_hora</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>alfanumerico</t>
+          <t>fecha</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Nombre completo del denunciante.</t>
+          <t>Hora de la denuncia.</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Lucía Sánchez</t>
+          <t>14:45</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>popolo:Person
- schema:Person</t>
+          <t>schema:Thing</t>
         </is>
       </c>
       <c r="H6" t="inlineStr"/>
@@ -606,12 +608,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Persona</t>
+          <t>Denuncia</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>denunciante_genero</t>
+          <t>denuncia_medio</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -621,20 +623,15 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Género según el cual se identifica la persona declarado según la normativa vigente para la presentación de declaraciones juradas en el país.</t>
+          <t>Indica de que forma fue realizada la denuncia</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Femenino</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>popolo:Person
- schema:Person</t>
-        </is>
-      </c>
+          <t>Página web</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
@@ -645,33 +642,28 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Persona</t>
+          <t>Denuncia</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>denunciante_edad</t>
+          <t>denuncia_lugar_radicacion</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>numerico</t>
+          <t>alfanumerico</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Edad al momento de la denuncia.</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
+          <t>Oficina o dependencia que recepciono la denuncia ya sea presencial, electrónica, telefónica u otro medio.</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
-          <t>popolo:Person
- schema:Person</t>
+          <t>schema:Thing</t>
         </is>
       </c>
       <c r="H8" t="inlineStr"/>
@@ -689,22 +681,22 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>denuncia_id</t>
+          <t>denuncia_enlace_seguimiento</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>alfanumerico</t>
+          <t>url</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Identificador de la denuncia realizada.</t>
+          <t>De existir un enlace para hacer seguimiento a la denuncia, opcional</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>3384556</t>
+          <t>https://www.bahia.gob.ar/vecinos/</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -727,29 +719,25 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>denuncia_fecha</t>
+          <t>denuncia_estado_actual</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>fecha</t>
+          <t>alfanumerico</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Fecha de la denuncia.</t>
+          <t>Ultimo estado de la denuncia</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2019-03-12</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>schema:Thing</t>
-        </is>
-      </c>
+          <t>Activo</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
     </row>
     <row r="11">
@@ -765,27 +753,27 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>denuncia_hora</t>
+          <t>denuncia_direccion</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>fecha</t>
+          <t>alfanumerico</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Hora de la denuncia.</t>
+          <t>Dirección donde sucedió el hecho denunciado.</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>Alsina 1600</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>schema:Thing</t>
+          <t>schema:PostalAddress</t>
         </is>
       </c>
       <c r="H11" t="inlineStr"/>
@@ -803,25 +791,29 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>denuncia_medio</t>
+          <t>denuncia_latitud</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>alfanumerico</t>
+          <t>numerico</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Indica de que forma fue realizada la denuncia</t>
+          <t>Latitud donde sucedió el hecho denunciado.</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Página web</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr"/>
+          <t>-38.705048</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>schema:GeoCoordinates</t>
+        </is>
+      </c>
       <c r="H12" t="inlineStr"/>
     </row>
     <row r="13">
@@ -837,23 +829,27 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>denuncia_lugar_radicacion</t>
+          <t>denuncia_longitud</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>alfanumerico</t>
+          <t>numerico</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Oficina o dependencia que recepciono la denuncia ya sea presencial, electrónica, telefónica u otro medio.</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr"/>
+          <t>Longitud donde sucedió el hecho denunciado.</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>-62.250596</t>
+        </is>
+      </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>schema:Thing</t>
+          <t>schema:GeoCoordinates</t>
         </is>
       </c>
       <c r="H13" t="inlineStr"/>
@@ -871,22 +867,22 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>denuncia_enlace_seguimiento</t>
+          <t>denuncia_detalle</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>url</t>
+          <t>texto</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>De existir un enlace para hacer seguimiento a la denuncia, opcional</t>
+          <t>Detalle brindado por el denunciante al realizar la denuncia.</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>https://www.bahia.gob.ar/vecinos/</t>
+          <t>Cable se encuentra colgando desde la columna de alumbrado.</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -909,7 +905,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>denuncia_estado_actual</t>
+          <t>denuncia_categoria</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -919,15 +915,19 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Ultimo estado de la denuncia</t>
+          <t>Categoría o clasificación del hecho denunciado.</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Activo</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr"/>
+          <t>Alumbrado</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>schema:Thing</t>
+        </is>
+      </c>
       <c r="H15" t="inlineStr"/>
     </row>
     <row r="16">
@@ -943,7 +943,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>denuncia_direccion</t>
+          <t>denuncia_tipo</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -953,17 +953,17 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Dirección donde sucedió el hecho denunciado.</t>
+          <t>Tipo de denuncia (esto es una clasificación más específica que "categoría").</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Alsina 1600</t>
+          <t>Cable Suelto</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>schema:PostalAddress</t>
+          <t>schema:Thing</t>
         </is>
       </c>
       <c r="H16" t="inlineStr"/>
@@ -981,27 +981,23 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>denuncia_latitud</t>
+          <t>denuncia_subtipo</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>numerico</t>
+          <t>alfanumerico</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Latitud donde sucedió el hecho denunciado.</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>-38.705048</t>
-        </is>
-      </c>
+          <t>Subtipo de denuncia (esto es una clasificación más específica que "tipo", si aplica).</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
         <is>
-          <t>schema:GeoCoordinates</t>
+          <t>schema:Thing</t>
         </is>
       </c>
       <c r="H17" t="inlineStr"/>
@@ -1019,27 +1015,23 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>denuncia_longitud</t>
+          <t>denuncia_otra_clasificacion</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>numerico</t>
+          <t>alfanumerico</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Longitud donde sucedió el hecho denunciado.</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>-62.250596</t>
-        </is>
-      </c>
+          <t>Categoría o clasificación alternativa del hecho denunciado.</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>schema:GeoCoordinates</t>
+          <t>schema:Thing</t>
         </is>
       </c>
       <c r="H18" t="inlineStr"/>
@@ -1057,27 +1049,27 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>denuncia_detalle</t>
+          <t>denuncia_fecha_ultimo_cambio</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>texto</t>
+          <t>fecha</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Detalle brindado por el denunciante al realizar la denuncia.</t>
+          <t>Fecha de la última modificación que sufrió la denuncia.</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Cable se encuentra colgando desde la columna de alumbrado.</t>
+          <t>2019-03-15</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>schema:Thing</t>
+          <t>schema:Date</t>
         </is>
       </c>
       <c r="H19" t="inlineStr"/>
@@ -1095,22 +1087,22 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>denuncia_categoria</t>
+          <t>denuncia_comentario_ultimo_cambio</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>alfanumerico</t>
+          <t>texto</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Categoría o clasificación del hecho denunciado.</t>
+          <t>Comentario agregado a la denuncia en el último cambio.</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Alumbrado</t>
+          <t>Se envió equipo a reparar el cable</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1119,188 +1111,6 @@
         </is>
       </c>
       <c r="H20" t="inlineStr"/>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Denuncias</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Denuncia</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>denuncia_tipo</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>alfanumerico</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Tipo de denuncia (esto es una clasificación más específica que "categoría").</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Cable Suelto</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>schema:Thing</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr"/>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Denuncias</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Denuncia</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>denuncia_subtipo</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>alfanumerico</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Subtipo de denuncia (esto es una clasificación más específica que "tipo", si aplica).</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>schema:Thing</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr"/>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Denuncias</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Denuncia</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>denuncia_otra_clasificacion</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>alfanumerico</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Categoría o clasificación alternativa del hecho denunciado.</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>schema:Thing</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr"/>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Denuncias</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Denuncia</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>denuncia_fecha_ultimo_cambio</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>fecha</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Fecha de la última modificación que sufrió la denuncia.</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>2019-03-15</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>schema:Date</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr"/>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Denuncias</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Denuncia</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>denuncia_comentario_ultimo_cambio</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>texto</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Comentario agregado a la denuncia en el último cambio.</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Se envió equipo a reparar el cable</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>schema:Thing</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>